<commit_message>
added research files for damage scaling. updates to npc and common object dat coming from study monster spell.
</commit_message>
<xml_diff>
--- a/File Research/CommonObjDat UW2.xlsx
+++ b/File Research/CommonObjDat UW2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D099F0A-9FFB-43C3-8CA0-B4CDB5764E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32D7295-EC11-483C-9560-DE4399F94179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{7ED1FA11-2114-4775-965F-EC4009C3E5C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="450">
   <si>
     <t>C5</t>
   </si>
@@ -1403,6 +1403,9 @@
     <t>Bit 4 
 Uses a detailed LookAt Description that begins with "You See" instead of just printing the object name</t>
   </si>
+  <si>
+    <t>Bit 1 Objects with this bit set will activate when in collision with another object</t>
+  </si>
 </sst>
 </file>
 
@@ -1898,14 +1901,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED46B61-4517-4515-9354-B9B0C7E0A8BB}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AP466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="K211" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="T20" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O217" sqref="O217"/>
+      <selection pane="bottomRight" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1930,7 +1932,7 @@
     <col min="21" max="21" width="5.19921875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.46484375" style="10" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.19921875" customWidth="1"/>
     <col min="25" max="25" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="2.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.53125" bestFit="1" customWidth="1"/>
@@ -2075,7 +2077,7 @@
         <v>428</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>426</v>
+        <v>449</v>
       </c>
       <c r="Y2" s="6" t="s">
         <v>424</v>
@@ -5269,7 +5271,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5426,7 +5428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5583,7 +5585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>22</v>
       </c>
@@ -5740,7 +5742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>23</v>
       </c>
@@ -6368,7 +6370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>27</v>
       </c>
@@ -6682,7 +6684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>29</v>
       </c>
@@ -6839,7 +6841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>30</v>
       </c>
@@ -12177,7 +12179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>64</v>
       </c>
@@ -12334,7 +12336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>65</v>
       </c>
@@ -12491,7 +12493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>66</v>
       </c>
@@ -12648,7 +12650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>67</v>
       </c>
@@ -12805,7 +12807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>68</v>
       </c>
@@ -12962,7 +12964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>69</v>
       </c>
@@ -13119,7 +13121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>70</v>
       </c>
@@ -13276,7 +13278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>71</v>
       </c>
@@ -13433,7 +13435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>72</v>
       </c>
@@ -13590,7 +13592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>73</v>
       </c>
@@ -13747,7 +13749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>74</v>
       </c>
@@ -13904,7 +13906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>75</v>
       </c>
@@ -14061,7 +14063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>76</v>
       </c>
@@ -14218,7 +14220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>77</v>
       </c>
@@ -14375,7 +14377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>78</v>
       </c>
@@ -14532,7 +14534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>79</v>
       </c>
@@ -14689,7 +14691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>80</v>
       </c>
@@ -14846,7 +14848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>81</v>
       </c>
@@ -15003,7 +15005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>82</v>
       </c>
@@ -15160,7 +15162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>83</v>
       </c>
@@ -15317,7 +15319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>84</v>
       </c>
@@ -15474,7 +15476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>85</v>
       </c>
@@ -15631,7 +15633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>86</v>
       </c>
@@ -15788,7 +15790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>87</v>
       </c>
@@ -15945,7 +15947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>88</v>
       </c>
@@ -16102,7 +16104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>89</v>
       </c>
@@ -16259,7 +16261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>90</v>
       </c>
@@ -16416,7 +16418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>91</v>
       </c>
@@ -16573,7 +16575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>92</v>
       </c>
@@ -16730,7 +16732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>93</v>
       </c>
@@ -16887,7 +16889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>94</v>
       </c>
@@ -17044,7 +17046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>95</v>
       </c>
@@ -17201,7 +17203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>96</v>
       </c>
@@ -17358,7 +17360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>97</v>
       </c>
@@ -17515,7 +17517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>98</v>
       </c>
@@ -17672,7 +17674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>99</v>
       </c>
@@ -17829,7 +17831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>100</v>
       </c>
@@ -17986,7 +17988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>101</v>
       </c>
@@ -18143,7 +18145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>102</v>
       </c>
@@ -18300,7 +18302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>103</v>
       </c>
@@ -18457,7 +18459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>104</v>
       </c>
@@ -18614,7 +18616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>105</v>
       </c>
@@ -18771,7 +18773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>106</v>
       </c>
@@ -18928,7 +18930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>107</v>
       </c>
@@ -19085,7 +19087,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>108</v>
       </c>
@@ -19242,7 +19244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>109</v>
       </c>
@@ -19399,7 +19401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>110</v>
       </c>
@@ -19556,7 +19558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>111</v>
       </c>
@@ -19713,7 +19715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>112</v>
       </c>
@@ -19870,7 +19872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>113</v>
       </c>
@@ -20027,7 +20029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>114</v>
       </c>
@@ -20184,7 +20186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>115</v>
       </c>
@@ -20341,7 +20343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>116</v>
       </c>
@@ -20498,7 +20500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>117</v>
       </c>
@@ -20655,7 +20657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>118</v>
       </c>
@@ -20812,7 +20814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>119</v>
       </c>
@@ -20969,7 +20971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>120</v>
       </c>
@@ -21126,7 +21128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>121</v>
       </c>
@@ -21283,7 +21285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>122</v>
       </c>
@@ -21440,7 +21442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>123</v>
       </c>
@@ -21597,7 +21599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>124</v>
       </c>
@@ -21754,7 +21756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>125</v>
       </c>
@@ -21911,7 +21913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>126</v>
       </c>
@@ -22068,7 +22070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>127</v>
       </c>
@@ -32273,7 +32275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>192</v>
       </c>
@@ -32430,7 +32432,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>193</v>
       </c>
@@ -34785,7 +34787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>208</v>
       </c>
@@ -34942,7 +34944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>209</v>
       </c>
@@ -35256,7 +35258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>211</v>
       </c>
@@ -35413,7 +35415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>212</v>
       </c>
@@ -35570,7 +35572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>213</v>
       </c>
@@ -35884,7 +35886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>215</v>
       </c>
@@ -36198,7 +36200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>217</v>
       </c>
@@ -36355,7 +36357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>218</v>
       </c>
@@ -36512,7 +36514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>219</v>
       </c>
@@ -36669,7 +36671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>220</v>
       </c>
@@ -36826,7 +36828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>221</v>
       </c>
@@ -36983,7 +36985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>222</v>
       </c>
@@ -37140,7 +37142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>223</v>
       </c>
@@ -37297,7 +37299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>224</v>
       </c>
@@ -44676,7 +44678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A274">
         <v>271</v>
       </c>
@@ -52369,7 +52371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="323" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A323">
         <v>320</v>
       </c>
@@ -52526,7 +52528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A324">
         <v>321</v>
       </c>
@@ -52683,7 +52685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A325">
         <v>322</v>
       </c>
@@ -52840,7 +52842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A326">
         <v>323</v>
       </c>
@@ -52997,7 +52999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A327">
         <v>324</v>
       </c>
@@ -53154,7 +53156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A328">
         <v>325</v>
       </c>
@@ -53311,7 +53313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A329">
         <v>326</v>
       </c>
@@ -53468,7 +53470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="330" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A330">
         <v>327</v>
       </c>
@@ -53625,7 +53627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="331" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A331">
         <v>328</v>
       </c>
@@ -53782,7 +53784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A332">
         <v>329</v>
       </c>
@@ -53939,7 +53941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A333">
         <v>330</v>
       </c>
@@ -54096,7 +54098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A334">
         <v>331</v>
       </c>
@@ -54253,7 +54255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A335">
         <v>332</v>
       </c>
@@ -54410,7 +54412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A336">
         <v>333</v>
       </c>
@@ -54567,7 +54569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A337">
         <v>334</v>
       </c>
@@ -54724,7 +54726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="338" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A338">
         <v>335</v>
       </c>
@@ -54881,7 +54883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="339" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A339">
         <v>336</v>
       </c>
@@ -55038,7 +55040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="340" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A340">
         <v>337</v>
       </c>
@@ -55195,7 +55197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A341">
         <v>338</v>
       </c>
@@ -55352,7 +55354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="342" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A342">
         <v>339</v>
       </c>
@@ -55509,7 +55511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="343" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A343">
         <v>340</v>
       </c>
@@ -55980,7 +55982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="346" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A346">
         <v>343</v>
       </c>
@@ -56137,7 +56139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="347" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A347">
         <v>344</v>
       </c>
@@ -56294,7 +56296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="348" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A348">
         <v>345</v>
       </c>
@@ -56451,7 +56453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="349" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A349">
         <v>346</v>
       </c>
@@ -56608,7 +56610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="350" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A350">
         <v>347</v>
       </c>
@@ -56765,7 +56767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A351">
         <v>348</v>
       </c>
@@ -56922,7 +56924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="352" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A352">
         <v>349</v>
       </c>
@@ -57079,7 +57081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A353">
         <v>350</v>
       </c>
@@ -57393,7 +57395,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="355" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A355">
         <v>352</v>
       </c>
@@ -57550,7 +57552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="356" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A356">
         <v>353</v>
       </c>
@@ -57707,7 +57709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="357" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A357">
         <v>354</v>
       </c>
@@ -57864,7 +57866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="358" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A358">
         <v>355</v>
       </c>
@@ -58021,7 +58023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="359" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A359">
         <v>356</v>
       </c>
@@ -58178,7 +58180,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="360" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A360">
         <v>357</v>
       </c>
@@ -58335,7 +58337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="361" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A361">
         <v>358</v>
       </c>
@@ -58492,7 +58494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="362" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A362">
         <v>359</v>
       </c>
@@ -58649,7 +58651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="363" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A363">
         <v>360</v>
       </c>
@@ -58806,7 +58808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="364" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A364">
         <v>361</v>
       </c>
@@ -58963,7 +58965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="365" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A365">
         <v>362</v>
       </c>
@@ -59120,7 +59122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A366">
         <v>363</v>
       </c>
@@ -59277,7 +59279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A367">
         <v>364</v>
       </c>
@@ -59434,7 +59436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="368" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A368">
         <v>365</v>
       </c>
@@ -59591,7 +59593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="369" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A369">
         <v>366</v>
       </c>
@@ -59748,7 +59750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="370" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A370">
         <v>367</v>
       </c>
@@ -59905,7 +59907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="371" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A371">
         <v>368</v>
       </c>
@@ -60062,7 +60064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="372" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A372">
         <v>369</v>
       </c>
@@ -60219,7 +60221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A373">
         <v>370</v>
       </c>
@@ -60376,7 +60378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A374">
         <v>371</v>
       </c>
@@ -60533,7 +60535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="375" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A375">
         <v>372</v>
       </c>
@@ -60690,7 +60692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="376" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A376">
         <v>373</v>
       </c>
@@ -60847,7 +60849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A377">
         <v>374</v>
       </c>
@@ -61004,7 +61006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A378">
         <v>375</v>
       </c>
@@ -61161,7 +61163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="379" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A379">
         <v>376</v>
       </c>
@@ -61318,7 +61320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="380" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A380">
         <v>377</v>
       </c>
@@ -61475,7 +61477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A381">
         <v>378</v>
       </c>
@@ -61632,7 +61634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="382" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A382">
         <v>379</v>
       </c>
@@ -61789,7 +61791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A383">
         <v>380</v>
       </c>
@@ -61946,7 +61948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="384" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A384">
         <v>381</v>
       </c>
@@ -62103,7 +62105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="385" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A385">
         <v>382</v>
       </c>
@@ -62260,7 +62262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="386" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A386">
         <v>383</v>
       </c>
@@ -62417,7 +62419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="387" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A387">
         <v>384</v>
       </c>
@@ -62574,7 +62576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="388" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A388">
         <v>385</v>
       </c>
@@ -62731,7 +62733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="389" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A389">
         <v>386</v>
       </c>
@@ -62888,7 +62890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="390" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A390">
         <v>387</v>
       </c>
@@ -63045,7 +63047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="391" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A391">
         <v>388</v>
       </c>
@@ -63202,7 +63204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="392" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A392">
         <v>389</v>
       </c>
@@ -63359,7 +63361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="393" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A393">
         <v>390</v>
       </c>
@@ -63516,7 +63518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="394" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A394">
         <v>391</v>
       </c>
@@ -63673,7 +63675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="395" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A395">
         <v>392</v>
       </c>
@@ -63830,7 +63832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="396" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A396">
         <v>393</v>
       </c>
@@ -63987,7 +63989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="397" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A397">
         <v>394</v>
       </c>
@@ -64144,7 +64146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="398" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A398">
         <v>395</v>
       </c>
@@ -64301,7 +64303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="399" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A399">
         <v>396</v>
       </c>
@@ -64458,7 +64460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="400" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A400">
         <v>397</v>
       </c>
@@ -64615,7 +64617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="401" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A401">
         <v>398</v>
       </c>
@@ -64772,7 +64774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="402" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A402">
         <v>399</v>
       </c>
@@ -64929,7 +64931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="403" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A403">
         <v>400</v>
       </c>
@@ -65086,7 +65088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="404" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A404">
         <v>401</v>
       </c>
@@ -65243,7 +65245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="405" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A405">
         <v>402</v>
       </c>
@@ -65400,7 +65402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="406" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A406">
         <v>403</v>
       </c>
@@ -65557,7 +65559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="407" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A407">
         <v>404</v>
       </c>
@@ -65714,7 +65716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="408" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A408">
         <v>405</v>
       </c>
@@ -65871,7 +65873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="409" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A409">
         <v>406</v>
       </c>
@@ -66028,7 +66030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="410" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="410" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A410">
         <v>407</v>
       </c>
@@ -66185,7 +66187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="411" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A411">
         <v>408</v>
       </c>
@@ -66342,7 +66344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="412" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A412">
         <v>409</v>
       </c>
@@ -66499,7 +66501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A413">
         <v>410</v>
       </c>
@@ -66656,7 +66658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A414">
         <v>411</v>
       </c>
@@ -66813,7 +66815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A415">
         <v>412</v>
       </c>
@@ -66970,7 +66972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A416">
         <v>413</v>
       </c>
@@ -67127,7 +67129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A417">
         <v>414</v>
       </c>
@@ -67284,7 +67286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="418" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A418">
         <v>415</v>
       </c>
@@ -67441,7 +67443,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="419" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A419">
         <v>416</v>
       </c>
@@ -67598,7 +67600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="420" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A420">
         <v>417</v>
       </c>
@@ -67755,7 +67757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="421" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A421">
         <v>418</v>
       </c>
@@ -67912,7 +67914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="422" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A422">
         <v>419</v>
       </c>
@@ -68069,7 +68071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="423" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A423">
         <v>420</v>
       </c>
@@ -68226,7 +68228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="424" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A424">
         <v>421</v>
       </c>
@@ -68383,7 +68385,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="425" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A425">
         <v>422</v>
       </c>
@@ -68540,7 +68542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="426" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A426">
         <v>423</v>
       </c>
@@ -68697,7 +68699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="427" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A427">
         <v>424</v>
       </c>
@@ -68854,7 +68856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="428" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A428">
         <v>425</v>
       </c>
@@ -69011,7 +69013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="429" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A429">
         <v>426</v>
       </c>
@@ -69168,7 +69170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="430" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A430">
         <v>427</v>
       </c>
@@ -69325,7 +69327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="431" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A431">
         <v>428</v>
       </c>
@@ -69482,7 +69484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="432" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A432">
         <v>429</v>
       </c>
@@ -69639,7 +69641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="433" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A433">
         <v>430</v>
       </c>
@@ -69796,7 +69798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="434" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="434" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A434">
         <v>431</v>
       </c>
@@ -69953,7 +69955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="435" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A435">
         <v>432</v>
       </c>
@@ -70110,7 +70112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="436" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="436" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A436">
         <v>433</v>
       </c>
@@ -70267,7 +70269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="437" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="437" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A437">
         <v>434</v>
       </c>
@@ -70424,7 +70426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="438" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="438" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A438">
         <v>435</v>
       </c>
@@ -70581,7 +70583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="439" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="439" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A439">
         <v>436</v>
       </c>
@@ -70738,7 +70740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="440" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="440" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A440">
         <v>437</v>
       </c>
@@ -70895,7 +70897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="441" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="441" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A441">
         <v>438</v>
       </c>
@@ -71052,7 +71054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="442" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="442" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A442">
         <v>439</v>
       </c>
@@ -71209,7 +71211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="443" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="443" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A443">
         <v>440</v>
       </c>
@@ -71366,7 +71368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="444" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="444" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A444">
         <v>441</v>
       </c>
@@ -71523,7 +71525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="445" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A445">
         <v>442</v>
       </c>
@@ -71680,7 +71682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="446" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="446" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A446">
         <v>443</v>
       </c>
@@ -71837,7 +71839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="447" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="447" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A447">
         <v>444</v>
       </c>
@@ -71994,7 +71996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="448" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A448">
         <v>445</v>
       </c>
@@ -72151,7 +72153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="449" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A449">
         <v>446</v>
       </c>
@@ -72308,7 +72310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="450" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="450" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A450">
         <v>447</v>
       </c>
@@ -72465,7 +72467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="451" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A451">
         <v>448</v>
       </c>
@@ -72622,7 +72624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="452" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="452" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A452">
         <v>449</v>
       </c>
@@ -72779,7 +72781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="453" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A453">
         <v>450</v>
       </c>
@@ -72936,7 +72938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="454" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="454" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A454">
         <v>451</v>
       </c>
@@ -73093,7 +73095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="455" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A455">
         <v>452</v>
       </c>
@@ -73250,7 +73252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="456" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="456" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A456">
         <v>453</v>
       </c>
@@ -73407,7 +73409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="457" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A457">
         <v>454</v>
       </c>
@@ -73564,7 +73566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="458" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="458" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A458">
         <v>455</v>
       </c>
@@ -73721,7 +73723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="459" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A459">
         <v>456</v>
       </c>
@@ -73878,7 +73880,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="460" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="460" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A460">
         <v>457</v>
       </c>
@@ -74035,7 +74037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="461" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A461">
         <v>458</v>
       </c>
@@ -74192,7 +74194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="462" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A462">
         <v>459</v>
       </c>
@@ -74349,7 +74351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="463" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A463">
         <v>460</v>
       </c>
@@ -74506,7 +74508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="464" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A464">
         <v>461</v>
       </c>
@@ -74663,7 +74665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="465" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A465">
         <v>462</v>
       </c>
@@ -74820,7 +74822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="466" spans="1:42" hidden="1" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A466">
         <v>463</v>
       </c>
@@ -74980,11 +74982,6 @@
   </sheetData>
   <autoFilter ref="A2:AP466" xr:uid="{CED46B61-4517-4515-9354-B9B0C7E0A8BB}">
     <filterColumn colId="6" showButton="0"/>
-    <filterColumn colId="14">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="18" showButton="0"/>
   </autoFilter>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Latest disassembly. Updated research spreadsheets
</commit_message>
<xml_diff>
--- a/File Research/CommonObjDat UW2.xlsx
+++ b/File Research/CommonObjDat UW2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77D5835-D475-4F6D-97B9-CC2855950FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCB6496-1332-4EA9-9256-A34ECCCB2DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="270" windowWidth="20505" windowHeight="12690" xr2:uid="{7ED1FA11-2114-4775-965F-EC4009C3E5C9}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="20640" windowHeight="13080" xr2:uid="{7ED1FA11-2114-4775-965F-EC4009C3E5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1384,10 +1384,6 @@
 Something to do with Raycasting</t>
   </si>
   <si>
-    <t>bits 1-4  (checked when object hits the ground, only set when object is a damaging projectile type so this is probability the missile is removed from the world on impact when Rng (0-7) is less thanthe value. Any value &gt;=8 means the projectile is destroyed on impact, 0 means object is not removed on impact.
-If the mobile object has bits 4,5,6 at offset 0xA set to 1 the projectile will be removed regardless of the below value and a splash spawned</t>
-  </si>
-  <si>
     <t>Bit 6/7 IsStackable or IsLinkable
 When 0 or 2 the object can be stacked into a quantity
 1 and 3 means the object can have a link</t>
@@ -1412,6 +1408,11 @@
   </si>
   <si>
     <t>bit 5,6,7,8</t>
+  </si>
+  <si>
+    <t>bits 1-4  culling priority for projectiles
+(checked when object hits the ground, only set when object is a damaging projectile type so this is probability the missile is removed from the world on impact when Rng (0-7) is less thanthe value. Any value of 9 means the projectile is destroyed on impact and cause damage in the tile, 0 means object is not removed on impact.
+If the mobile object has bits 4,5,6 at offset 0xA set to 1 the projectile will be removed regardless of the below value and a splash spawned</t>
   </si>
 </sst>
 </file>
@@ -1908,13 +1909,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED46B61-4517-4515-9354-B9B0C7E0A8BB}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AR466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z2" sqref="Z2"/>
+      <selection pane="bottomRight" activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2024,7 +2026,7 @@
       <c r="AQ1" s="13"/>
       <c r="AR1" s="13"/>
     </row>
-    <row r="2" spans="1:44" s="3" customFormat="1" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:44" s="3" customFormat="1" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>389</v>
       </c>
@@ -2060,13 +2062,13 @@
         <v>383</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>429</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>428</v>
@@ -2085,16 +2087,16 @@
         <v>385</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Y2" s="6" t="s">
         <v>427</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AA2" s="6" t="s">
         <v>423</v>
@@ -2107,7 +2109,7 @@
         <v>443</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>386</v>
@@ -2143,10 +2145,10 @@
         <v>388</v>
       </c>
       <c r="AQ2" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AR2" s="12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.45">
@@ -4788,7 +4790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>16</v>
       </c>
@@ -4953,7 +4955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5118,7 +5120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5283,7 +5285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5448,7 +5450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5613,7 +5615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5778,7 +5780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>22</v>
       </c>
@@ -5943,7 +5945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>23</v>
       </c>
@@ -6603,7 +6605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>27</v>
       </c>
@@ -6768,7 +6770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>28</v>
       </c>
@@ -6933,7 +6935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>29</v>
       </c>
@@ -7098,7 +7100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>30</v>
       </c>
@@ -57753,7 +57755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="340" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A340">
         <v>337</v>
       </c>
@@ -57918,7 +57920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:44" hidden="1" x14ac:dyDescent="0.45">
       <c r="A341">
         <v>338</v>
       </c>
@@ -78712,6 +78714,11 @@
   <autoFilter ref="A2:AR466" xr:uid="{CED46B61-4517-4515-9354-B9B0C7E0A8BB}">
     <filterColumn colId="6" showButton="0"/>
     <filterColumn colId="18" showButton="0"/>
+    <filterColumn colId="30">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <mergeCells count="10">
     <mergeCell ref="AB1:AE1"/>

</xml_diff>